<commit_message>
Ampie modifiche jxls e nuovo use case
</commit_message>
<xml_diff>
--- a/templates/CovidToscana.xlsx
+++ b/templates/CovidToscana.xlsx
@@ -301,8 +301,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Colore 2" xfId="2" builtinId="35"/>
@@ -435,11 +437,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="319364432"/>
-        <c:axId val="319366208"/>
+        <c:axId val="624461776"/>
+        <c:axId val="319116624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="319364432"/>
+        <c:axId val="624461776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -482,7 +484,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319366208"/>
+        <c:crossAx val="319116624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -490,7 +492,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="319366208"/>
+        <c:axId val="319116624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +543,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="319364432"/>
+        <c:crossAx val="624461776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -997,11 +999,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="398562496"/>
-        <c:axId val="343536640"/>
+        <c:axId val="318962048"/>
+        <c:axId val="752024672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="398562496"/>
+        <c:axId val="318962048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1044,7 +1046,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343536640"/>
+        <c:crossAx val="752024672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1052,7 +1054,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="343536640"/>
+        <c:axId val="752024672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1102,7 +1104,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="398562496"/>
+        <c:crossAx val="318962048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2763,15 +2765,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>566614</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>24420</xdr:rowOff>
+      <xdr:colOff>160214</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>710220</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>507999</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:colOff>101599</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>101599</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2818,6 +2820,43 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1181101</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1879600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>822217</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Immagine 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:srcRect r="62741"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9982201" y="88900"/>
+          <a:ext cx="698499" cy="733317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3148,7 +3187,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3160,8 +3199,8 @@
     <col min="7" max="7" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:7" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="13"/>
@@ -3173,25 +3212,25 @@
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New template for CovidToscana.xlsx
</commit_message>
<xml_diff>
--- a/templates/CovidToscana.xlsx
+++ b/templates/CovidToscana.xlsx
@@ -1,24 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francescogradi/Desktop/ExportLibrary-BackEnd/templates/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A2CE44-0506-204C-B1E8-C7D97D447080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="Result" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="ActiveCases">Template!$G$4</definedName>
+    <definedName name="DailyCases">Template!$B$4</definedName>
+    <definedName name="Deaths">Template!$E$4</definedName>
+    <definedName name="GlobalCases">Template!$C$4</definedName>
+    <definedName name="IntensiveCases">Template!$F$4</definedName>
+    <definedName name="Recovered">Template!$D$4</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,12 +41,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Autore</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,13 +70,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -72,12 +85,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="fields" var="province" lastCell="G4")</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jx:each(items="fields" var="province" lastCell="G4")</t>
         </r>
       </text>
     </comment>
@@ -86,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -168,16 +190,25 @@
   <si>
     <t>Active Cases</t>
   </si>
+  <si>
+    <t>Num prov:</t>
+  </si>
+  <si>
+    <t>Valori:</t>
+  </si>
+  <si>
+    <t>${numProvince}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +264,19 @@
       <sz val="20"/>
       <color theme="0"/>
       <name val="Calibri (Corpo)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -317,12 +361,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -336,7 +383,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -418,14 +464,19 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C272-9A42-8644-8612E33A95B1}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -593,7 +644,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -607,7 +658,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -662,6 +712,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F048-BE44-8994-C3470B1246A9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -677,6 +732,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-F048-BE44-8994-C3470B1246A9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -692,6 +752,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-F048-BE44-8994-C3470B1246A9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -707,6 +772,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-F048-BE44-8994-C3470B1246A9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -786,13 +856,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Template!$D$14,Template!$E$14,Template!$F$14,Template!$G$14)</c:f>
+              <c:f>(Template!$I$26,Template!$J$26,Template!$K$26,Template!$L$26)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-F048-BE44-8994-C3470B1246A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
@@ -816,7 +903,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -884,7 +970,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -898,7 +984,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -980,14 +1065,19 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2E79-8943-B106-15116AB33BCE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1074,6 +1164,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2747,7 +2838,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Grafico 3"/>
+        <xdr:cNvPr id="4" name="Grafico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2777,7 +2874,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Grafico 4"/>
+        <xdr:cNvPr id="5" name="Grafico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2807,7 +2910,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Grafico 5"/>
+        <xdr:cNvPr id="6" name="Grafico 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2837,7 +2946,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Immagine 1"/>
+        <xdr:cNvPr id="2" name="Immagine 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3183,11 +3298,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3267,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="12">
-        <f t="shared" si="0"/>
+        <f>SUM(C4)</f>
         <v>0</v>
       </c>
       <c r="D5" s="12">
@@ -3284,6 +3399,35 @@
       </c>
       <c r="G5" s="12" t="e">
         <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="25" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" t="e">
+        <f ca="1">OFFSET(D4, I25, 0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J26" t="e">
+        <f ca="1">OFFSET(E4, I25, 0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K26" t="e">
+        <f ca="1">OFFSET(F4, I25, 0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L26" t="e">
+        <f ca="1">OFFSET(G4, I25, 0)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3296,8 +3440,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E9"/>

</xml_diff>

<commit_message>
Dynamic charts are now working
</commit_message>
<xml_diff>
--- a/templates/CovidToscana.xlsx
+++ b/templates/CovidToscana.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A2CE44-0506-204C-B1E8-C7D97D447080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5FDB1D-1AAB-BA4E-AF2B-4F0CBFAF8A6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -61,12 +61,31 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="G6")</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">jx:area(lastCell="I26")
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>")</t>
         </r>
       </text>
     </comment>
@@ -100,6 +119,30 @@
             <family val="2"/>
           </rPr>
           <t>jx:each(items="fields" var="province" lastCell="G4")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I25" authorId="0" shapeId="0" xr:uid="{75827B33-1B41-BF4D-8148-1886CA66AFBF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Autore:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jx:each(items="fields" var="province" lastCell="I26")</t>
         </r>
       </text>
     </comment>
@@ -197,7 +240,7 @@
     <t>Valori:</t>
   </si>
   <si>
-    <t>${numProvince}</t>
+    <t>${province.numProvince}</t>
   </si>
 </sst>
 </file>
@@ -208,7 +251,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,17 +267,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -274,6 +311,19 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -327,28 +377,29 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Colore 2" xfId="2" builtinId="35"/>
@@ -856,7 +907,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Template!$I$26,Template!$J$26,Template!$K$26,Template!$L$26)</c:f>
+              <c:f>(Template!$M$26,Template!$N$26,Template!$O$26,Template!$P$26)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2861,16 +2912,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>160214</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>490414</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>710220</xdr:rowOff>
+      <xdr:rowOff>684820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>101599</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>431799</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>101599</xdr:rowOff>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3299,10 +3350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3312,9 +3363,11 @@
     <col min="4" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.5" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>12</v>
       </c>
@@ -3325,8 +3378,8 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
@@ -3345,11 +3398,11 @@
       <c r="F3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
@@ -3372,13 +3425,14 @@
         <f>C4 - D4 - E4 - F4</f>
         <v>#VALUE!</v>
       </c>
+      <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="12">
-        <f t="shared" ref="B5:G5" si="0">SUM(B4)</f>
+        <f t="shared" ref="B5:E5" si="0">SUM(B4)</f>
         <v>0</v>
       </c>
       <c r="C5" s="12">
@@ -3394,39 +3448,39 @@
         <v>0</v>
       </c>
       <c r="F5" s="12">
-        <f t="shared" si="0"/>
+        <f>SUM(F4)</f>
         <v>0</v>
       </c>
       <c r="G5" s="12" t="e">
-        <f t="shared" si="0"/>
+        <f>SUM(G4)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="25" spans="8:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="8:16" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
         <v>27</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="8:12" x14ac:dyDescent="0.2">
-      <c r="H26" t="s">
+    <row r="26" spans="8:16" x14ac:dyDescent="0.2">
+      <c r="L26" t="s">
         <v>28</v>
       </c>
-      <c r="I26" t="e">
+      <c r="M26" t="e">
         <f ca="1">OFFSET(D4, I25, 0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="J26" t="e">
+      <c r="N26" t="e">
         <f ca="1">OFFSET(E4, I25, 0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K26" t="e">
+      <c r="O26" t="e">
         <f ca="1">OFFSET(F4, I25, 0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="L26" t="e">
+      <c r="P26" t="e">
         <f ca="1">OFFSET(G4, I25, 0)</f>
         <v>#VALUE!</v>
       </c>

</xml_diff>

<commit_message>
Modifiche varie nomi e templates
</commit_message>
<xml_diff>
--- a/templates/CovidToscana.xlsx
+++ b/templates/CovidToscana.xlsx
@@ -9,19 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
-    <sheet name="Result" sheetId="2" r:id="rId2"/>
+    <sheet name="Daily Cases" sheetId="2" r:id="rId2"/>
+    <sheet name="Global Cases" sheetId="4" r:id="rId3"/>
+    <sheet name="Summary" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ActiveCases">Template!$G$4</definedName>
-    <definedName name="DailyCases">Template!$B$4</definedName>
-    <definedName name="Deaths">Template!$E$4</definedName>
-    <definedName name="GlobalCases">Template!$C$4</definedName>
-    <definedName name="IntensiveCases">Template!$F$4</definedName>
-    <definedName name="Recovered">Template!$D$4</definedName>
+    <definedName name="ActiveCases">Template!$G$5</definedName>
+    <definedName name="DailyCases">Template!$B$5</definedName>
+    <definedName name="Deaths">Template!$E$5</definedName>
+    <definedName name="GlobalCases">Template!$C$5</definedName>
+    <definedName name="IntensiveCases">Template!$F$5</definedName>
+    <definedName name="Recovered">Template!$D$5</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -74,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0">
+    <comment ref="A5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -94,16 +96,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>jx:each(items="fields" var="province" lastCell="G4")</t>
+jx:each(items="fields" var="province" lastCell="G5")</t>
         </r>
       </text>
     </comment>
@@ -112,43 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Birth Date</t>
-  </si>
-  <si>
-    <t>Payment</t>
-  </si>
-  <si>
-    <t>Bonus</t>
-  </si>
-  <si>
-    <t>Summary:</t>
-  </si>
-  <si>
-    <t>Total Payment</t>
-  </si>
-  <si>
-    <t>Excel Formulas Demo</t>
-  </si>
-  <si>
-    <t>Elsa</t>
-  </si>
-  <si>
-    <t>Oleg</t>
-  </si>
-  <si>
-    <t>Neil</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Covid Toscana</t>
   </si>
@@ -194,27 +151,21 @@
   <si>
     <t>Active Cases</t>
   </si>
-  <si>
-    <t>Num prov:</t>
-  </si>
-  <si>
-    <t>Valori:</t>
-  </si>
-  <si>
-    <t>${numProvince}</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -249,15 +200,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -283,24 +225,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -331,35 +261,50 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Colore 2" xfId="2" builtinId="35"/>
     <cellStyle name="Colore 2" xfId="1" builtinId="33"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -379,14 +324,39 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="104"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="4"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="3000"/>
+              <a:t>Daily Cases</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -429,7 +399,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Template!$B$3</c:f>
+              <c:f>Template!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -440,7 +410,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -450,38 +420,27 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Template!$A$4:$A$13</c:f>
+              <c:f>Template!$A$5:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>${province.province}</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Tuscany:</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Template!$B$4:$B$13</c:f>
+              <c:f>Template!$B$5:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="0">
                   <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C272-9A42-8644-8612E33A95B1}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -491,18 +450,73 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-1551797600"/>
-        <c:axId val="-1551781968"/>
+        <c:gapWidth val="0"/>
+        <c:axId val="1073818160"/>
+        <c:axId val="1074647888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1551797600"/>
+        <c:axId val="1073818160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="3000"/>
+                  <a:t>Provinces</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -540,7 +554,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1551781968"/>
+        <c:crossAx val="1074647888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -548,28 +562,69 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1551781968"/>
+        <c:axId val="1074647888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="3000"/>
+                  <a:t>Cases</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -599,7 +654,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1551797600"/>
+        <c:crossAx val="1073818160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -655,6 +710,398 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="3000"/>
+              <a:t>Global Cases</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Template!$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Global Cases</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Template!$A$5:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>${province.province}</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Template!$C$5:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2E79-8943-B106-15116AB33BCE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:axId val="1119632832"/>
+        <c:axId val="1119226480"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1119632832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="3000"/>
+                  <a:t>Provinces</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1119226480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1119226480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="it-IT" sz="3000"/>
+                  <a:t>Cases</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1119632832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
@@ -663,6 +1110,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="3200"/>
+              <a:t>Tuscany Global Cases</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -844,7 +1316,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>(Template!$D$3,Template!$E$3,Template!$F$3,Template!$G$3)</c:f>
+              <c:f>(Template!$D$4,Template!$E$4,Template!$F$4,Template!$G$4)</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -864,9 +1336,9 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Template!$I$26,Template!$J$26,Template!$K$26,Template!$L$26)</c:f>
+              <c:f>(Template!$D$3,Template!$E$3,Template!$F$3,Template!$G$3)</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
@@ -911,6 +1383,29 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="2100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -925,7 +1420,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -978,289 +1473,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="103"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="3"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Template!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Global Cases</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Template!$A$4:$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>${province.province}</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Tuscany:</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Template!$C$4:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2E79-8943-B106-15116AB33BCE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-1505630320"/>
-        <c:axId val="-1505627568"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-1505630320"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1505627568"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-1505627568"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-1505630320"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
-  <a:schemeClr val="accent2"/>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1300,9 +1513,49 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="21">
   <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -1810,7 +2063,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1867,7 +2120,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1918,13 +2171,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -1935,19 +2181,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -1985,7 +2224,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -2028,23 +2267,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2149,8 +2387,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2282,20 +2520,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2329,7 +2566,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2386,7 +2623,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2437,6 +2674,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2447,12 +2691,19 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -2490,7 +2741,7 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -2533,22 +2784,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2653,8 +2905,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2786,19 +3038,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2833,114 +3086,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>152202</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>92340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>752230</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>146537</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Grafico 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>160214</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>710220</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>101599</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>101599</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Grafico 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1012092</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>86946</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1285631</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>149469</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Grafico 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -2959,7 +3104,7 @@
         <xdr:cNvPr id="2" name="Immagine 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2968,7 +3113,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:srcRect r="62741"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -2985,6 +3130,147 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabella2" displayName="Tabella2" ref="A4:G5" totalsRowShown="0" headerRowCellStyle="40% - Colore 2">
+  <autoFilter ref="A4:G5"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Province" dataDxfId="6"/>
+    <tableColumn id="2" name="Daily Cases" dataDxfId="5"/>
+    <tableColumn id="3" name="Global Cases" dataDxfId="4"/>
+    <tableColumn id="4" name="Recovered" dataDxfId="3"/>
+    <tableColumn id="5" name="Deaths" dataDxfId="2"/>
+    <tableColumn id="6" name="Intensive Cares" dataDxfId="1"/>
+    <tableColumn id="7" name="Active Cases" dataDxfId="0">
+      <calculatedColumnFormula>C5 - D5 - E5 - F5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3309,10 +3595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3325,119 +3611,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>12</v>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>14</v>
+      <c r="B3" s="4">
+        <f>SUM(B5)</f>
+        <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>15</v>
+      <c r="C3" s="4">
+        <f>SUM(C5)</f>
+        <v>0</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>19</v>
+      <c r="D3" s="4">
+        <f>SUM(D5)</f>
+        <v>0</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>21</v>
+      <c r="E3" s="4">
+        <f>SUM(E5)</f>
+        <v>0</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>23</v>
+      <c r="F3" s="4">
+        <f>SUM(F5)</f>
+        <v>0</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="11" t="e">
-        <f>C4 - D4 - E4 - F4</f>
+      <c r="G3" s="4" t="e">
+        <f>SUM(G5)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>25</v>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
       </c>
-      <c r="B5" s="12">
-        <f t="shared" ref="B5:G5" si="0">SUM(B4)</f>
-        <v>0</v>
+      <c r="B4" s="6" t="s">
+        <v>2</v>
       </c>
-      <c r="C5" s="12">
-        <f>SUM(C4)</f>
-        <v>0</v>
+      <c r="C4" s="6" t="s">
+        <v>3</v>
       </c>
-      <c r="D5" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="D4" s="6" t="s">
+        <v>7</v>
       </c>
-      <c r="E5" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
       </c>
-      <c r="F5" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
       </c>
-      <c r="G5" s="12" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+      <c r="G4" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="25" spans="8:12" x14ac:dyDescent="0.2">
-      <c r="H25" t="s">
-        <v>27</v>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
       </c>
-      <c r="I25" t="s">
-        <v>29</v>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="8:12" x14ac:dyDescent="0.2">
-      <c r="H26" t="s">
-        <v>28</v>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
       </c>
-      <c r="I26" t="e">
-        <f ca="1">OFFSET(D4, I25, 0)</f>
-        <v>#VALUE!</v>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
       </c>
-      <c r="J26" t="e">
-        <f ca="1">OFFSET(E4, I25, 0)</f>
-        <v>#VALUE!</v>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
       </c>
-      <c r="K26" t="e">
-        <f ca="1">OFFSET(F4, I25, 0)</f>
-        <v>#VALUE!</v>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
       </c>
-      <c r="L26" t="e">
-        <f ca="1">OFFSET(G4, I25, 0)</f>
+      <c r="G5" s="3" t="e">
+        <f>C5 - D5 - E5 - F5</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3446,6 +3703,9 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -3454,10 +3714,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3469,139 +3729,87 @@
     <col min="5" max="5" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4">
-        <v>25759</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1500</v>
-      </c>
-      <c r="D4" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="E4" s="5">
-        <f>C4*(1+D4)</f>
-        <v>1724.9999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>26784</v>
-      </c>
-      <c r="C5" s="5">
-        <v>2300</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="E5" s="5">
-        <f>C5*(1+D5)</f>
-        <v>2875</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="4">
-        <v>27672</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2500</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <f>C6*(1+D6)</f>
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4">
-        <v>28497</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1700</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0.15</v>
-      </c>
-      <c r="E7" s="5">
-        <f>C7*(1+D7)</f>
-        <v>1954.9999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="4">
-        <v>25353</v>
-      </c>
-      <c r="C8" s="5">
-        <v>2800</v>
-      </c>
-      <c r="D8" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="E8" s="5">
-        <f>C8*(1+D8)</f>
-        <v>3360</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7">
-        <f>SUM(C4:C8)</f>
-        <v>10800</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7">
-        <f>SUM(E4:E8)</f>
-        <v>12415</v>
-      </c>
-    </row>
+    <row r="1" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>